<commit_message>
This is a excel file about USA housing
</commit_message>
<xml_diff>
--- a/QMBE Advanced BA.xlsx
+++ b/QMBE Advanced BA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendanebel/Desktop/QMBE_3730_BrendanEbel_2025/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendanebel/Desktop/QMBE_3730_BrendanEbel_2025/QMBE_3730_BrendanEbel_2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F793466-CAE9-7A4D-9DDA-42149439D505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA0EAD8-A73A-D843-9F7C-17CA8DCAFCC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16360" xr2:uid="{1FA2734B-DD84-154E-8B63-4148164BB9C9}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340" xr2:uid="{1FA2734B-DD84-154E-8B63-4148164BB9C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Brendan Ebel</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -407,7 +415,13 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>